<commit_message>
Adjust the constants and restart new experiment with 100 and 50 percentage values
</commit_message>
<xml_diff>
--- a/second-semester/src/data analyse.xlsx
+++ b/second-semester/src/data analyse.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungh\Desktop\msc-project\second-semester\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5151B7C-0C3D-4028-B730-75C80B55AB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CCF02D-54A7-416D-BD60-768D4E693762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3780" yWindow="-20745" windowWidth="18285" windowHeight="15825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9645" yWindow="-19650" windowWidth="18975" windowHeight="15825" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="63">
   <si>
     <t>Thinking Time (ms)</t>
   </si>
@@ -183,6 +184,51 @@
   <si>
     <t xml:space="preserve">(MParanoid,2,100) </t>
   </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>250ms time limit</t>
+  </si>
+  <si>
+    <t>500ms time limit</t>
+  </si>
+  <si>
+    <t>1000ms time limit</t>
+  </si>
+  <si>
+    <t>MP100</t>
+  </si>
+  <si>
+    <t>MB100</t>
+  </si>
+  <si>
+    <t>MP50</t>
+  </si>
+  <si>
+    <t>MB50</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with time limit of 500ms</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with time limit of 1000ms</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with iterations limit of 100</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with iterations limit of 50</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with time limit of 250ms</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with time limit of 750ms</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game with iterations limit of 10</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,6 +304,12 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,6 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -549,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,24 +621,24 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -620,7 +673,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -644,7 +697,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>500</v>
       </c>
@@ -666,7 +719,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>1000</v>
       </c>
@@ -697,7 +750,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1">
@@ -721,7 +774,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1">
         <v>500</v>
       </c>
@@ -743,7 +796,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1">
         <v>1000</v>
       </c>
@@ -774,7 +827,7 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1">
@@ -798,7 +851,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1">
         <v>500</v>
       </c>
@@ -820,7 +873,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1">
         <v>1000</v>
       </c>
@@ -851,7 +904,7 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1">
@@ -875,7 +928,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1">
         <v>500</v>
       </c>
@@ -897,7 +950,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1">
         <v>1000</v>
       </c>
@@ -919,24 +972,24 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
@@ -972,7 +1025,7 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="1">
@@ -996,7 +1049,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1">
         <v>500</v>
       </c>
@@ -1018,7 +1071,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1">
         <v>1000</v>
       </c>
@@ -1049,7 +1102,7 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="1">
@@ -1073,7 +1126,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1">
         <v>500</v>
       </c>
@@ -1095,7 +1148,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1">
         <v>1000</v>
       </c>
@@ -1126,7 +1179,7 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1">
@@ -1150,7 +1203,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="1">
         <v>500</v>
       </c>
@@ -1172,7 +1225,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="1">
         <v>1000</v>
       </c>
@@ -1203,7 +1256,7 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1">
@@ -1227,7 +1280,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="1">
         <v>500</v>
       </c>
@@ -1249,7 +1302,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="1">
         <v>1000</v>
       </c>
@@ -1271,24 +1324,24 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
@@ -1324,7 +1377,7 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="1">
@@ -1348,7 +1401,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="1">
         <v>500</v>
       </c>
@@ -1370,7 +1423,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="1">
         <v>1000</v>
       </c>
@@ -1401,7 +1454,7 @@
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B50" s="1">
@@ -1425,7 +1478,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="1">
         <v>500</v>
       </c>
@@ -1447,7 +1500,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="1">
         <v>1000</v>
       </c>
@@ -1478,7 +1531,7 @@
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B54" s="1">
@@ -1502,7 +1555,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="1">
         <v>500</v>
       </c>
@@ -1524,7 +1577,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="1">
         <v>1000</v>
       </c>
@@ -1555,7 +1608,7 @@
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="1">
@@ -1579,7 +1632,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
+      <c r="A59" s="9"/>
       <c r="B59" s="1">
         <v>500</v>
       </c>
@@ -1601,7 +1654,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="1">
         <v>1000</v>
       </c>
@@ -1623,24 +1676,24 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
@@ -1676,7 +1729,7 @@
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B66" s="1">
@@ -1700,7 +1753,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="7"/>
+      <c r="A67" s="9"/>
       <c r="B67" s="1">
         <v>500</v>
       </c>
@@ -1722,7 +1775,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="7"/>
+      <c r="A68" s="9"/>
       <c r="B68" s="1">
         <v>1000</v>
       </c>
@@ -1753,7 +1806,7 @@
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="1">
@@ -1777,7 +1830,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="7"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="1">
         <v>500</v>
       </c>
@@ -1799,7 +1852,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="7"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="1">
         <v>1000</v>
       </c>
@@ -1830,7 +1883,7 @@
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B74" s="1">
@@ -1854,7 +1907,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="7"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="1">
         <v>500</v>
       </c>
@@ -1876,7 +1929,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="7"/>
+      <c r="A76" s="9"/>
       <c r="B76" s="1">
         <v>1000</v>
       </c>
@@ -1907,7 +1960,7 @@
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B78" s="1">
@@ -1931,7 +1984,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="7"/>
+      <c r="A79" s="9"/>
       <c r="B79" s="1">
         <v>500</v>
       </c>
@@ -1953,7 +2006,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A80" s="7"/>
+      <c r="A80" s="9"/>
       <c r="B80" s="1">
         <v>1000</v>
       </c>
@@ -1975,24 +2028,24 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
@@ -2028,7 +2081,7 @@
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="1">
@@ -2052,7 +2105,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="7"/>
+      <c r="A87" s="9"/>
       <c r="B87" s="1">
         <v>500</v>
       </c>
@@ -2074,7 +2127,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="7"/>
+      <c r="A88" s="9"/>
       <c r="B88" s="1">
         <v>1000</v>
       </c>
@@ -2105,7 +2158,7 @@
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B90" s="1">
@@ -2129,7 +2182,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="7"/>
+      <c r="A91" s="9"/>
       <c r="B91" s="1">
         <v>500</v>
       </c>
@@ -2151,7 +2204,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="7"/>
+      <c r="A92" s="9"/>
       <c r="B92" s="1">
         <v>1000</v>
       </c>
@@ -2182,7 +2235,7 @@
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B94" s="1">
@@ -2206,7 +2259,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="7"/>
+      <c r="A95" s="9"/>
       <c r="B95" s="1">
         <v>500</v>
       </c>
@@ -2228,7 +2281,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="7"/>
+      <c r="A96" s="9"/>
       <c r="B96" s="1">
         <v>1000</v>
       </c>
@@ -2259,7 +2312,7 @@
       <c r="H97" s="1"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B98" s="1">
@@ -2283,7 +2336,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="7"/>
+      <c r="A99" s="9"/>
       <c r="B99" s="1">
         <v>500</v>
       </c>
@@ -2305,7 +2358,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="7"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="1">
         <v>1000</v>
       </c>
@@ -2327,24 +2380,24 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="8" t="s">
+      <c r="A102" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C103" s="9" t="s">
+      <c r="C103" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
-      <c r="F103" s="9"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B104" s="1" t="s">
@@ -2380,7 +2433,7 @@
       <c r="H105" s="1"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B106" s="1">
@@ -2404,7 +2457,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="7"/>
+      <c r="A107" s="9"/>
       <c r="B107" s="1">
         <v>500</v>
       </c>
@@ -2426,7 +2479,7 @@
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="7"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="1">
         <v>1000</v>
       </c>
@@ -2457,7 +2510,7 @@
       <c r="H109" s="1"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B110" s="1">
@@ -2481,7 +2534,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="7"/>
+      <c r="A111" s="9"/>
       <c r="B111" s="1">
         <v>500</v>
       </c>
@@ -2503,7 +2556,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="7"/>
+      <c r="A112" s="9"/>
       <c r="B112" s="1">
         <v>1000</v>
       </c>
@@ -2534,7 +2587,7 @@
       <c r="H113" s="1"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B114" s="1">
@@ -2558,7 +2611,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="7"/>
+      <c r="A115" s="9"/>
       <c r="B115" s="1">
         <v>500</v>
       </c>
@@ -2580,7 +2633,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="7"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="1">
         <v>1000</v>
       </c>
@@ -2611,7 +2664,7 @@
       <c r="H117" s="1"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B118" s="1">
@@ -2635,7 +2688,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="7"/>
+      <c r="A119" s="9"/>
       <c r="B119" s="1">
         <v>500</v>
       </c>
@@ -2657,7 +2710,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="7"/>
+      <c r="A120" s="9"/>
       <c r="B120" s="1">
         <v>1000</v>
       </c>
@@ -2679,24 +2732,24 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A122" s="8" t="s">
+      <c r="A122" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B122" s="8"/>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8"/>
-      <c r="H122" s="8"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C123" s="9" t="s">
+      <c r="C123" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B124" s="1" t="s">
@@ -2732,7 +2785,7 @@
       <c r="H125" s="1"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="7" t="s">
+      <c r="A126" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B126" s="1">
@@ -2756,7 +2809,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="7"/>
+      <c r="A127" s="9"/>
       <c r="B127" s="1">
         <v>500</v>
       </c>
@@ -2778,7 +2831,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="7"/>
+      <c r="A128" s="9"/>
       <c r="B128" s="1">
         <v>1000</v>
       </c>
@@ -2809,7 +2862,7 @@
       <c r="H129" s="1"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="7" t="s">
+      <c r="A130" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B130" s="1">
@@ -2833,7 +2886,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A131" s="7"/>
+      <c r="A131" s="9"/>
       <c r="B131" s="1">
         <v>500</v>
       </c>
@@ -2855,7 +2908,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A132" s="7"/>
+      <c r="A132" s="9"/>
       <c r="B132" s="1">
         <v>1000</v>
       </c>
@@ -2886,7 +2939,7 @@
       <c r="H133" s="1"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="7" t="s">
+      <c r="A134" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B134" s="1">
@@ -2910,7 +2963,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="7"/>
+      <c r="A135" s="9"/>
       <c r="B135" s="1">
         <v>500</v>
       </c>
@@ -2932,7 +2985,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A136" s="7"/>
+      <c r="A136" s="9"/>
       <c r="B136" s="1">
         <v>1000</v>
       </c>
@@ -2963,7 +3016,7 @@
       <c r="H137" s="1"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="7" t="s">
+      <c r="A138" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B138" s="1">
@@ -2987,7 +3040,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A139" s="7"/>
+      <c r="A139" s="9"/>
       <c r="B139" s="1">
         <v>500</v>
       </c>
@@ -3009,7 +3062,7 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="7"/>
+      <c r="A140" s="9"/>
       <c r="B140" s="1">
         <v>1000</v>
       </c>
@@ -3032,20 +3085,18 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A126:A128"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="A114:A116"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A122:H122"/>
-    <mergeCell ref="C123:F123"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A102:H102"/>
-    <mergeCell ref="C103:F103"/>
-    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="C63:F63"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A82:H82"/>
     <mergeCell ref="C83:F83"/>
@@ -3062,18 +3113,20 @@
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A74:A76"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="C63:F63"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A102:H102"/>
+    <mergeCell ref="C103:F103"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A126:A128"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A122:H122"/>
+    <mergeCell ref="C123:F123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3083,8 +3136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81735FC2-F85C-4056-8A81-27EBDFB0EE35}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H17"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3102,24 +3155,24 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -3145,7 +3198,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -3169,7 +3222,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>1000</v>
       </c>
@@ -3191,7 +3244,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>1500</v>
       </c>
@@ -3213,7 +3266,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1">
@@ -3237,7 +3290,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1">
         <v>1000</v>
       </c>
@@ -3259,7 +3312,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1">
         <v>1500</v>
       </c>
@@ -3281,7 +3334,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1">
@@ -3305,7 +3358,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1">
         <v>1000</v>
       </c>
@@ -3327,7 +3380,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="1">
         <v>1500</v>
       </c>
@@ -3349,7 +3402,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1">
@@ -3373,7 +3426,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1">
         <v>1000</v>
       </c>
@@ -3395,7 +3448,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1">
         <v>1500</v>
       </c>
@@ -3417,24 +3470,24 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
@@ -3460,7 +3513,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="1">
@@ -3480,7 +3533,7 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1">
         <v>1000</v>
       </c>
@@ -3498,7 +3551,7 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1">
         <v>1500</v>
       </c>
@@ -3516,7 +3569,7 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="1">
@@ -3536,7 +3589,7 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="1">
         <v>1000</v>
       </c>
@@ -3554,7 +3607,7 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1">
         <v>1500</v>
       </c>
@@ -3572,7 +3625,7 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="1">
@@ -3592,7 +3645,7 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="1">
         <v>1000</v>
       </c>
@@ -3610,7 +3663,7 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="1">
         <v>1500</v>
       </c>
@@ -3628,7 +3681,7 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="1">
@@ -3648,7 +3701,7 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1">
         <v>1000</v>
       </c>
@@ -3666,7 +3719,7 @@
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="1">
         <v>1500</v>
       </c>
@@ -3684,24 +3737,24 @@
       <c r="H33" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
@@ -3727,7 +3780,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="1">
@@ -3741,7 +3794,7 @@
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="1">
         <v>1000</v>
       </c>
@@ -3753,7 +3806,7 @@
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="1">
         <v>1500</v>
       </c>
@@ -3765,7 +3818,7 @@
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B41" s="1">
@@ -3779,7 +3832,7 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="1">
         <v>1000</v>
       </c>
@@ -3791,7 +3844,7 @@
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="1">
         <v>1500</v>
       </c>
@@ -3803,7 +3856,7 @@
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="1">
@@ -3817,7 +3870,7 @@
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="1">
         <v>1000</v>
       </c>
@@ -3829,7 +3882,7 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="1">
         <v>1500</v>
       </c>
@@ -3841,7 +3894,7 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B47" s="1">
@@ -3855,7 +3908,7 @@
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="1">
         <v>1000</v>
       </c>
@@ -3867,7 +3920,7 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="1">
         <v>1500</v>
       </c>
@@ -3879,24 +3932,24 @@
       <c r="H49" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
@@ -3922,7 +3975,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B55" s="1">
@@ -3936,7 +3989,7 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="1">
         <v>1000</v>
       </c>
@@ -3948,7 +4001,7 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
+      <c r="A57" s="9"/>
       <c r="B57" s="1">
         <v>1500</v>
       </c>
@@ -3960,7 +4013,7 @@
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="1">
@@ -3974,7 +4027,7 @@
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
+      <c r="A59" s="9"/>
       <c r="B59" s="1">
         <v>1000</v>
       </c>
@@ -3986,7 +4039,7 @@
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="1">
         <v>1500</v>
       </c>
@@ -3998,7 +4051,7 @@
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B61" s="1">
@@ -4012,7 +4065,7 @@
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="7"/>
+      <c r="A62" s="9"/>
       <c r="B62" s="1">
         <v>1000</v>
       </c>
@@ -4024,7 +4077,7 @@
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="7"/>
+      <c r="A63" s="9"/>
       <c r="B63" s="1">
         <v>1500</v>
       </c>
@@ -4036,7 +4089,7 @@
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B64" s="1">
@@ -4050,7 +4103,7 @@
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="7"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="1">
         <v>1000</v>
       </c>
@@ -4062,7 +4115,7 @@
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="7"/>
+      <c r="A66" s="9"/>
       <c r="B66" s="1">
         <v>1500</v>
       </c>
@@ -4075,6 +4128,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A55:A57"/>
     <mergeCell ref="A58:A60"/>
     <mergeCell ref="A61:A63"/>
@@ -4084,21 +4152,6 @@
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="A52:H52"/>
     <mergeCell ref="C53:F53"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4106,10 +4159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEDF561-454D-45FB-90EE-3F7E5DF036BA}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4123,9 +4176,10 @@
     <col min="8" max="8" width="13.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="15.5546875" customWidth="1"/>
-    <col min="11" max="11" width="18.21875" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -4159,13 +4213,13 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
       <c r="H4" t="s">
         <v>28</v>
       </c>
@@ -4207,7 +4261,7 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -4231,7 +4285,7 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>500</v>
       </c>
@@ -4257,7 +4311,7 @@
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>1000</v>
       </c>
@@ -4300,7 +4354,7 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1">
@@ -4328,7 +4382,7 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1">
         <v>500</v>
       </c>
@@ -4354,7 +4408,7 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1">
         <v>1000</v>
       </c>
@@ -4397,7 +4451,7 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
@@ -4428,7 +4482,7 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1">
         <v>500</v>
       </c>
@@ -4453,7 +4507,7 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1">
         <v>1000</v>
       </c>
@@ -4481,16 +4535,10 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="C17" s="6">
-        <f xml:space="preserve"> AVERAGE(C14:C16)</f>
-        <v>0.48299999999999993</v>
-      </c>
-      <c r="D17" s="6">
-        <f xml:space="preserve"> AVERAGE(D14:D16)</f>
-        <v>0.49866666666666665</v>
-      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
       <c r="G17" s="3"/>
@@ -4504,8 +4552,8 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1">
@@ -4531,8 +4579,8 @@
       <c r="L18" s="1"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
       <c r="B19" s="1">
         <v>500</v>
       </c>
@@ -4556,8 +4604,8 @@
       <c r="L19" s="1"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
       <c r="B20" s="1">
         <v>1000</v>
       </c>
@@ -4581,15 +4629,9 @@
       <c r="L20" s="1"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C21" s="6">
-        <f xml:space="preserve"> AVERAGE(C18:C20)</f>
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="D21" s="6">
-        <f xml:space="preserve"> AVERAGE(D18:D20)</f>
-        <v>0.48666666666666664</v>
-      </c>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="G21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="1"/>
@@ -4597,17 +4639,20 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="G22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -4620,22 +4665,41 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C24" s="9" t="s">
+      <c r="K23" s="7"/>
+      <c r="L23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="H24" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="N24" s="8">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
@@ -4657,11 +4721,21 @@
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="5"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="K25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.30299999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="1">
@@ -4678,11 +4752,21 @@
       <c r="G26" s="3"/>
       <c r="I26" s="1"/>
       <c r="J26" s="3"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="K26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.505</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
       <c r="B27" s="1">
         <v>500</v>
       </c>
@@ -4697,12 +4781,21 @@
       <c r="G27" s="3"/>
       <c r="I27" s="1"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="K27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
       <c r="B28" s="1">
         <v>1000</v>
       </c>
@@ -4717,11 +4810,20 @@
       <c r="G28" s="3"/>
       <c r="I28" s="1"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="8">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="N28" s="8">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -4730,12 +4832,21 @@
       <c r="G29" s="3"/>
       <c r="I29" s="1"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="K29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.438</v>
+      </c>
+      <c r="M29" s="6">
+        <v>0.505</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0.309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="1">
@@ -4752,12 +4863,21 @@
       <c r="G30" s="3"/>
       <c r="I30" s="1"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="3"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="K30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.496</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0.317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
       <c r="B31" s="1">
         <v>500</v>
       </c>
@@ -4772,12 +4892,21 @@
       <c r="G31" s="3"/>
       <c r="I31" s="1"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="K31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
       <c r="B32" s="1">
         <v>1000</v>
       </c>
@@ -4796,7 +4925,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -4805,12 +4934,15 @@
       <c r="G33" s="3"/>
       <c r="I33" s="1"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="K33" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="1">
@@ -4832,12 +4964,19 @@
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
       <c r="B35" s="1">
         <v>500</v>
       </c>
@@ -4857,12 +4996,21 @@
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="3"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="K35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
       <c r="B36" s="1">
         <v>1000</v>
       </c>
@@ -4882,31 +5030,43 @@
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="3"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="M36" s="8">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="N36" s="8">
+        <v>0.317</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
-      <c r="C37" s="6">
-        <f xml:space="preserve"> AVERAGE(C34:C36)</f>
-        <v>0.45633333333333331</v>
-      </c>
-      <c r="D37" s="6">
-        <f xml:space="preserve"> AVERAGE(D34:D36)</f>
-        <v>0.48966666666666664</v>
-      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="3"/>
       <c r="I37" s="1"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="K37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L37" s="8">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="1">
@@ -4928,12 +5088,21 @@
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="3"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="K38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0.30199999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
       <c r="B39" s="1">
         <v>500</v>
       </c>
@@ -4953,12 +5122,21 @@
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="3"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="K39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39" s="8">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="M39" s="8">
+        <v>0.497</v>
+      </c>
+      <c r="N39" s="8">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
       <c r="B40" s="1">
         <v>1000</v>
       </c>
@@ -4978,36 +5156,60 @@
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="3"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="N40" s="1">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
-      <c r="C41" s="6">
-        <f xml:space="preserve"> AVERAGE(C38:C40)</f>
-        <v>0.47066666666666662</v>
-      </c>
-      <c r="D41" s="6">
-        <f xml:space="preserve"> AVERAGE(D38:D40)</f>
-        <v>0.49399999999999999</v>
-      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="N41" s="1">
+        <v>0.29299999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="3"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0.495</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>32</v>
       </c>
@@ -5021,18 +5223,20 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C44" s="9" t="s">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
       <c r="H44" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K44" s="5"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>22</v>
       </c>
@@ -5054,11 +5258,15 @@
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="5"/>
-      <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+      <c r="K45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="1">
@@ -5075,11 +5283,19 @@
       <c r="G46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="3"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="3"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
       <c r="B47" s="1">
         <v>500</v>
       </c>
@@ -5094,12 +5310,21 @@
       <c r="G47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="3"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
+      <c r="K47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L47" s="8">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="M47" s="8">
+        <v>0.504</v>
+      </c>
+      <c r="N47" s="1">
+        <v>0.31900000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
       <c r="B48" s="1">
         <v>1000</v>
       </c>
@@ -5114,11 +5339,20 @@
       <c r="G48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="3"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="M48" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="N48" s="8">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -5127,12 +5361,21 @@
       <c r="G49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="3"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+      <c r="K49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="N49" s="1">
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B50" s="1">
@@ -5149,12 +5392,21 @@
       <c r="G50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="3"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="3"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
+      <c r="K50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L50" s="1">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="M50" s="1">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="N50" s="8">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
       <c r="B51" s="1">
         <v>500</v>
       </c>
@@ -5169,12 +5421,21 @@
       <c r="G51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="3"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
+      <c r="K51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L51" s="8">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="N51" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
       <c r="B52" s="1">
         <v>1000</v>
       </c>
@@ -5189,11 +5450,20 @@
       <c r="G52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="3"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L52" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5202,11 +5472,21 @@
       <c r="G53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="K53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L53" s="1">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="M53" s="8">
+        <v>0.495</v>
+      </c>
+      <c r="N53" s="8">
+        <v>0.32400000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="1">
@@ -5228,11 +5508,21 @@
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
+      <c r="K54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="M54" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="N54" s="1">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
       <c r="B55" s="1">
         <v>500</v>
       </c>
@@ -5255,8 +5545,8 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
       <c r="B56" s="1">
         <v>1000</v>
       </c>
@@ -5279,16 +5569,10 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
-      <c r="C57" s="6">
-        <f xml:space="preserve"> AVERAGE(C54:C56)</f>
-        <v>0.47899999999999993</v>
-      </c>
-      <c r="D57" s="6">
-        <f xml:space="preserve"> AVERAGE(D54:D56)</f>
-        <v>0.48900000000000005</v>
-      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="3"/>
@@ -5297,8 +5581,8 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B58" s="1">
@@ -5323,8 +5607,8 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
       <c r="B59" s="1">
         <v>500</v>
       </c>
@@ -5347,8 +5631,8 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
       <c r="B60" s="1">
         <v>1000</v>
       </c>
@@ -5371,23 +5655,13 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C61" s="6">
-        <f xml:space="preserve"> AVERAGE(C58:C60)</f>
-        <v>0.46233333333333332</v>
-      </c>
-      <c r="D61" s="6">
-        <f xml:space="preserve"> AVERAGE(D58:D60)</f>
-        <v>0.49366666666666664</v>
-      </c>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
       <c r="G61" s="3"/>
       <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K62" s="1"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>34</v>
       </c>
@@ -5401,13 +5675,13 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C64" s="9" t="s">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C64" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
       <c r="H64" t="s">
         <v>28</v>
       </c>
@@ -5435,7 +5709,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B66" s="1">
@@ -5452,7 +5726,7 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="7"/>
+      <c r="A67" s="9"/>
       <c r="B67" s="1">
         <v>500</v>
       </c>
@@ -5467,7 +5741,7 @@
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="7"/>
+      <c r="A68" s="9"/>
       <c r="B68" s="1">
         <v>1000</v>
       </c>
@@ -5490,7 +5764,7 @@
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="1">
@@ -5507,7 +5781,7 @@
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="7"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="1">
         <v>500</v>
       </c>
@@ -5522,7 +5796,7 @@
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="7"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="1">
         <v>1000</v>
       </c>
@@ -5545,7 +5819,7 @@
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B74" s="1">
@@ -5567,7 +5841,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="7"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="1">
         <v>500</v>
       </c>
@@ -5587,7 +5861,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="7"/>
+      <c r="A76" s="9"/>
       <c r="B76" s="1">
         <v>1000</v>
       </c>
@@ -5608,20 +5882,14 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
-      <c r="C77" s="6">
-        <f xml:space="preserve"> AVERAGE(C74:C76)</f>
-        <v>0.47333333333333333</v>
-      </c>
-      <c r="D77" s="6">
-        <f xml:space="preserve"> AVERAGE(D74:D76)</f>
-        <v>0.47399999999999998</v>
-      </c>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B78" s="1">
@@ -5643,7 +5911,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="7"/>
+      <c r="A79" s="9"/>
       <c r="B79" s="1">
         <v>500</v>
       </c>
@@ -5663,7 +5931,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A80" s="7"/>
+      <c r="A80" s="9"/>
       <c r="B80" s="1">
         <v>1000</v>
       </c>
@@ -5683,18 +5951,22 @@
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C81" s="6">
-        <f xml:space="preserve"> AVERAGE(C78:C80)</f>
-        <v>0.46933333333333332</v>
-      </c>
-      <c r="D81" s="6">
-        <f xml:space="preserve"> AVERAGE(D78:D80)</f>
-        <v>0.47633333333333328</v>
-      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
       <c r="G81" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C44:F44"/>
@@ -5708,15 +5980,620 @@
     <mergeCell ref="A58:A60"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D33FE-1D44-4ACB-8B96-6B9822BF387F}">
+  <dimension ref="A1:O37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="I21" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="1"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+      <c r="I26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="I27" s="2"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="I28" s="2"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update part of the experiment data
</commit_message>
<xml_diff>
--- a/second-semester/src/data analyse.xlsx
+++ b/second-semester/src/data analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungh\Desktop\msc-project\second-semester\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD58C97-A9E0-4DD3-BF3F-6125ED2572E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1408F655-9C36-47C1-94CA-2F63B582858A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="-21600" windowWidth="19410" windowHeight="21705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9320" yWindow="-21600" windowWidth="19380" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
   <si>
     <t>Move</t>
   </si>
@@ -110,7 +110,40 @@
     <t>Constant: C = 0.1, W = 5.0</t>
   </si>
   <si>
-    <t>Unknown</t>
+    <t>MBRS</t>
+  </si>
+  <si>
+    <t>Lookup Table</t>
+  </si>
+  <si>
+    <t>MP50</t>
+  </si>
+  <si>
+    <t>MB50</t>
+  </si>
+  <si>
+    <t>MP10</t>
+  </si>
+  <si>
+    <t>MB10</t>
+  </si>
+  <si>
+    <t>MParanoid10</t>
+  </si>
+  <si>
+    <t>MBRS10</t>
+  </si>
+  <si>
+    <t>Win rate of three-player game against Random and Move-based player</t>
+  </si>
+  <si>
+    <t>Time cost (s) for 1000 playouts</t>
+  </si>
+  <si>
+    <t>Playouts performed within certain time</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -198,48 +231,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,23 +556,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D33FE-1D44-4ACB-8B96-6B9822BF387F}">
-  <dimension ref="A1:W57"/>
+  <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
     <col min="14" max="14" width="10.88671875" customWidth="1"/>
     <col min="15" max="15" width="10.33203125" customWidth="1"/>
   </cols>
@@ -562,7 +599,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="5"/>
@@ -572,24 +609,21 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1"/>
       <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
       <c r="P4" s="6"/>
       <c r="Q4" t="s">
         <v>9</v>
@@ -607,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
@@ -615,7 +649,7 @@
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="1"/>
@@ -627,54 +661,56 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="N5" s="6"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="9" t="s">
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16">
         <v>0.46700000000000003</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="16">
         <v>0.45800000000000002</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="16">
         <v>0.52100000000000002</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="G6" s="16">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="H6" s="18">
         <f xml:space="preserve"> AVERAGE(C6:G6)</f>
-        <v>0.48200000000000004</v>
+        <v>0.49725000000000008</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="16">
         <v>0.29640718562874202</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="16">
         <v>0.34131736526946099</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="16">
         <v>0.36227544910179599</v>
       </c>
-      <c r="N6" s="3"/>
+      <c r="N6" s="20"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="1" t="s">
@@ -693,38 +729,40 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16">
         <v>0.45400000000000001</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="16">
         <v>0.46500000000000002</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="16">
         <v>0.52500000000000002</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
-        <f t="shared" ref="H7:H21" si="0" xml:space="preserve"> AVERAGE(C7:G7)</f>
-        <v>0.48133333333333334</v>
+      <c r="G7" s="16">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="H7" s="18">
+        <f t="shared" ref="H7:H24" si="0" xml:space="preserve"> AVERAGE(C7:G7)</f>
+        <v>0.49675000000000002</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="16">
         <v>0.28343313373253398</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="16">
         <v>0.380239520958083</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="16">
         <v>0.33632734530938102</v>
       </c>
-      <c r="N7" s="3"/>
+      <c r="N7" s="20"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="1">
@@ -743,38 +781,40 @@
       <c r="V7" s="1"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16">
         <v>0.45100000000000001</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="16">
         <v>0.46300000000000002</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="16">
         <v>0.50600000000000001</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
+      <c r="G8" s="16">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="H8" s="18">
         <f t="shared" si="0"/>
-        <v>0.47333333333333333</v>
+        <v>0.48224999999999996</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="16">
         <v>0.29441117764470998</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="16">
         <v>0.370259481037924</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="16">
         <v>0.33532934131736503</v>
       </c>
-      <c r="N8" s="3"/>
+      <c r="N8" s="20"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="1">
@@ -793,44 +833,46 @@
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16">
         <v>0.44</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="16">
         <v>0.442</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="16">
         <v>0.52900000000000003</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
+      <c r="G9" s="16">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="H9" s="18">
         <f t="shared" si="0"/>
-        <v>0.47033333333333333</v>
+        <v>0.48825000000000002</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="16">
         <v>0.29840319361277401</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="16">
         <v>0.33133732534930099</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="16">
         <v>0.370259481037924</v>
       </c>
-      <c r="N9" s="3"/>
+      <c r="N9" s="20"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="1">
         <v>0.3</v>
       </c>
-      <c r="R9" s="15">
+      <c r="R9" s="9">
         <v>0.54200000000000004</v>
       </c>
       <c r="S9" s="1">
@@ -843,32 +885,45 @@
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="16">
         <v>0.53300000000000003</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16">
         <v>0.51200000000000001</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="16">
         <v>0.56499999999999995</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
+      <c r="G10" s="16">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="H10" s="18">
         <f t="shared" si="0"/>
-        <v>0.53666666666666663</v>
+        <v>0.54449999999999998</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="J10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="23">
+        <f xml:space="preserve"> AVERAGE(K6:K9)</f>
+        <v>0.29316367265469001</v>
+      </c>
+      <c r="L10" s="23">
+        <f t="shared" ref="L10:M10" si="1" xml:space="preserve"> AVERAGE(L6:L9)</f>
+        <v>0.35578842315369225</v>
+      </c>
+      <c r="M10" s="23">
+        <f t="shared" si="1"/>
+        <v>0.35104790419161652</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="1">
@@ -885,36 +940,33 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="16">
         <v>0.54600000000000004</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16">
         <v>0.505</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="16">
         <v>0.58399999999999996</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3">
+      <c r="G11" s="16">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="H11" s="18">
         <f t="shared" si="0"/>
-        <v>0.54500000000000004</v>
+        <v>0.54350000000000009</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="20"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="1">
@@ -931,121 +983,126 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="16">
         <v>0.54900000000000004</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16">
         <v>0.51700000000000002</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="16">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3">
+      <c r="G12" s="16">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="H12" s="18">
         <f t="shared" si="0"/>
-        <v>0.53866666666666674</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0.30738522954091801</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0.40219560878243499</v>
-      </c>
-      <c r="M12" s="3">
-        <v>0.290419161676646</v>
-      </c>
+        <v>0.54875000000000007</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="20"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="16">
         <v>0.55600000000000005</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
         <v>0.51500000000000001</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="16">
         <v>0.57699999999999996</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="3">
+      <c r="G13" s="16">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="H13" s="18">
         <f t="shared" si="0"/>
-        <v>0.54933333333333334</v>
-      </c>
-      <c r="I13" s="12"/>
+        <v>0.56025000000000003</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="J13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.30139720558882199</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0.41916167664670601</v>
-      </c>
-      <c r="M13" s="3">
-        <v>0.279441117764471</v>
-      </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="K13" s="16">
+        <v>0.30738522954091801</v>
+      </c>
+      <c r="L13" s="16">
+        <v>0.40219560878243499</v>
+      </c>
+      <c r="M13" s="16">
+        <v>0.290419161676646</v>
+      </c>
+      <c r="N13" s="20"/>
+      <c r="O13" s="5"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="9" t="s">
+      <c r="Q13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="16">
         <v>0.54200000000000004</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="16">
         <v>0.48799999999999999</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3">
+      <c r="E14" s="16"/>
+      <c r="F14" s="16">
         <v>0.55400000000000005</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="3">
+      <c r="G14" s="16">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="H14" s="18">
         <f t="shared" si="0"/>
-        <v>0.52800000000000002</v>
+        <v>0.53125</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0.30239520958083799</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0.37524950099800303</v>
-      </c>
-      <c r="M14" s="3">
-        <v>0.32235528942115699</v>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="K14" s="16">
+        <v>0.30139720558882199</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0.41916167664670601</v>
+      </c>
+      <c r="M14" s="16">
+        <v>0.279441117764471</v>
+      </c>
+      <c r="N14" s="20"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
       <c r="Q14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1060,39 +1117,41 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="16">
         <v>0.53500000000000003</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="16">
         <v>0.495</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3">
+      <c r="E15" s="16"/>
+      <c r="F15" s="16">
         <v>0.53200000000000003</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
+      <c r="G15" s="16">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="H15" s="18">
         <f t="shared" si="0"/>
-        <v>0.52066666666666672</v>
+        <v>0.52875000000000005</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0.319361277445109</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0.39321357285429098</v>
-      </c>
-      <c r="M15" s="3">
-        <v>0.28742514970059801</v>
-      </c>
-      <c r="N15" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.30239520958083799</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0.37524950099800303</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0.32235528942115699</v>
+      </c>
+      <c r="N15" s="20"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="1">
@@ -1109,31 +1168,41 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="16">
         <v>0.53700000000000003</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="16">
         <v>0.48299999999999998</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16">
         <v>0.55700000000000005</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3">
+      <c r="G16" s="16">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="H16" s="18">
         <f t="shared" si="0"/>
-        <v>0.52566666666666662</v>
+        <v>0.54099999999999993</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="J16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="16">
+        <v>0.319361277445109</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0.39321357285429098</v>
+      </c>
+      <c r="M16" s="16">
+        <v>0.28742514970059801</v>
+      </c>
+      <c r="N16" s="20"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="1">
@@ -1150,37 +1219,50 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="16">
         <v>0.55800000000000005</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="16">
         <v>0.48499999999999999</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3">
+      <c r="G17" s="16">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="H17" s="18">
         <f t="shared" si="0"/>
-        <v>0.53766666666666663</v>
+        <v>0.53774999999999995</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="J17" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="23">
+        <f xml:space="preserve"> AVERAGE(K13:K16)</f>
+        <v>0.30763473053892176</v>
+      </c>
+      <c r="L17" s="23">
+        <f t="shared" ref="L17:M17" si="2" xml:space="preserve"> AVERAGE(L13:L16)</f>
+        <v>0.39745508982035871</v>
+      </c>
+      <c r="M17" s="23">
+        <f t="shared" si="2"/>
+        <v>0.29491017964071797</v>
+      </c>
+      <c r="N17" s="20"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="1">
         <v>0.3</v>
       </c>
-      <c r="R17" s="15">
+      <c r="R17" s="9">
         <v>0.53300000000000003</v>
       </c>
       <c r="S17" s="1">
@@ -1191,33 +1273,35 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="16">
         <v>0.47899999999999998</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="16">
         <v>0.435</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="16">
         <v>0.44600000000000001</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3">
+      <c r="F18" s="16"/>
+      <c r="G18" s="16">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="H18" s="18">
         <f t="shared" si="0"/>
-        <v>0.45333333333333331</v>
+        <v>0.46824999999999994</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="20"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="1">
@@ -1234,26 +1318,39 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="16">
         <v>0.47499999999999998</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="16">
         <v>0.41599999999999998</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="16">
         <v>0.46800000000000003</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3">
+      <c r="F19" s="16"/>
+      <c r="G19" s="16">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="H19" s="18">
         <f t="shared" si="0"/>
-        <v>0.45300000000000001</v>
+        <v>0.46825</v>
       </c>
       <c r="I19" s="2"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="20"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="1">
@@ -1270,81 +1367,125 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="21" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="16">
         <v>0.49399999999999999</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="16">
         <v>0.45</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="16">
         <v>0.443</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="H20" s="18">
         <f t="shared" si="0"/>
-        <v>0.46233333333333332</v>
+        <v>0.47425</v>
       </c>
       <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.33532934131736503</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.390219560878243</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.27445109780439098</v>
+      </c>
+      <c r="N20" s="20"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="16">
         <v>0.47399999999999998</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="16">
         <v>0.42299999999999999</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="16">
         <v>0.43</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="H21" s="18">
         <f t="shared" si="0"/>
-        <v>0.4423333333333333</v>
-      </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="19"/>
+        <v>0.45250000000000001</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="16">
+        <v>0.300399201596806</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0.42115768463073799</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0.27844311377245501</v>
+      </c>
+      <c r="N21" s="20"/>
+      <c r="O21" s="10"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
+      <c r="C22" s="19">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="D22" s="19">
+        <v>0.432</v>
+      </c>
+      <c r="E22" s="19">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="F22" s="19">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="18">
+        <f t="shared" si="0"/>
+        <v>0.45874999999999999</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="16">
+        <v>0.35828343313373201</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0.38822355289421101</v>
+      </c>
+      <c r="M22" s="16">
+        <v>0.25349301397205498</v>
+      </c>
+      <c r="N22" s="20"/>
+      <c r="O22" s="5"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -1352,44 +1493,87 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="14"/>
+      <c r="B23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="11"/>
+      <c r="C23" s="19">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="D23" s="19">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="E23" s="19">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="18">
+        <f t="shared" si="0"/>
+        <v>0.46274999999999999</v>
+      </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
+      <c r="J23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="16">
+        <v>0.29940119760479</v>
+      </c>
+      <c r="L23" s="16">
+        <v>0.40618762475049902</v>
+      </c>
+      <c r="M23" s="16">
+        <v>0.29441117764470998</v>
+      </c>
+      <c r="N23" s="20"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="21" t="s">
+      <c r="A24" s="14"/>
+      <c r="B24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="3"/>
+      <c r="C24" s="19">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D24" s="19">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="E24" s="19">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="F24" s="19">
+        <v>0.49</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="18">
+        <f t="shared" si="0"/>
+        <v>0.45374999999999999</v>
+      </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
+      <c r="J24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="23">
+        <f xml:space="preserve"> AVERAGE(K20:K23)</f>
+        <v>0.32335329341317326</v>
+      </c>
+      <c r="L24" s="23">
+        <f xml:space="preserve"> AVERAGE(L20:L23)</f>
+        <v>0.40144710578842274</v>
+      </c>
+      <c r="M24" s="23">
+        <f xml:space="preserve"> AVERAGE(M20:M23)</f>
+        <v>0.27519960079840278</v>
+      </c>
+      <c r="N24" s="20"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="1"/>
@@ -1398,21 +1582,33 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
+      <c r="C25" s="19">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="D25" s="19">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="E25" s="19">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="18">
+        <f xml:space="preserve"> AVERAGE(C25:G25)</f>
+        <v>0.46099999999999997</v>
+      </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="20"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="1"/>
@@ -1421,8 +1617,6 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1430,10 +1624,16 @@
       <c r="G26" s="3"/>
       <c r="I26" s="2"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="20"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="1"/>
@@ -1442,19 +1642,25 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="3"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
+      <c r="J27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="16">
+        <v>0.30339321357285398</v>
+      </c>
+      <c r="L27" s="16">
+        <v>0.37125748502993999</v>
+      </c>
+      <c r="M27" s="16">
+        <v>0.32534930139720503</v>
+      </c>
+      <c r="N27" s="20"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="1"/>
@@ -1463,38 +1669,59 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
       <c r="G28" s="3"/>
       <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="16">
+        <v>0.300399201596806</v>
+      </c>
+      <c r="L28" s="16">
+        <v>0.36826347305389201</v>
+      </c>
+      <c r="M28" s="16">
+        <v>0.33133732534930099</v>
+      </c>
+      <c r="N28" s="20"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
       <c r="G29" s="3"/>
       <c r="I29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="16">
+        <v>0.249500998003992</v>
+      </c>
+      <c r="L29" s="16">
+        <v>0.40818363273453001</v>
+      </c>
+      <c r="M29" s="16">
+        <v>0.34231536926147699</v>
+      </c>
+      <c r="N29" s="20"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
       <c r="G30" s="3"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="19"/>
+      <c r="J30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="16">
+        <v>0.31536926147704503</v>
+      </c>
+      <c r="L30" s="16">
+        <v>0.35628742514970002</v>
+      </c>
+      <c r="M30" s="16">
+        <v>0.32834331337325301</v>
+      </c>
+      <c r="N30" s="20"/>
+      <c r="O30" s="10"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="1" t="s">
         <v>4</v>
@@ -1510,20 +1737,29 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" s="23">
+        <f xml:space="preserve"> AVERAGE(K27:K30)</f>
+        <v>0.29216566866267424</v>
+      </c>
+      <c r="L31" s="23">
+        <f t="shared" ref="L31:M31" si="3" xml:space="preserve"> AVERAGE(L27:L30)</f>
+        <v>0.37599800399201555</v>
+      </c>
+      <c r="M31" s="23">
+        <f t="shared" si="3"/>
+        <v>0.33183632734530899</v>
+      </c>
+      <c r="N31" s="20"/>
+      <c r="O31" s="5"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="1">
         <v>0.1</v>
@@ -1533,387 +1769,910 @@
         <v>0.14200000000000002</v>
       </c>
       <c r="S31" s="1">
-        <f t="shared" ref="S31:T31" si="1" xml:space="preserve"> ABS(S7-S15)</f>
+        <f t="shared" ref="S31:T31" si="4" xml:space="preserve"> ABS(S7-S15)</f>
         <v>1.7000000000000015E-2</v>
       </c>
       <c r="T31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.19199999999999995</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="11"/>
+      <c r="A32" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="17"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
       <c r="Q32" s="1">
         <v>0.2</v>
       </c>
       <c r="R32" s="1">
-        <f t="shared" ref="R32:T32" si="2" xml:space="preserve"> ABS(R8-R16)</f>
+        <f t="shared" ref="R32:T32" si="5" xml:space="preserve"> ABS(R8-R16)</f>
         <v>6.6999999999999948E-2</v>
       </c>
       <c r="S32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.4999999999999967E-2</v>
       </c>
       <c r="T32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="3"/>
+      <c r="B33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="I33" s="2"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="20"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="1">
         <v>0.3</v>
       </c>
       <c r="R33" s="7">
-        <f t="shared" ref="R33:T33" si="3" xml:space="preserve"> ABS(R9-R17)</f>
+        <f t="shared" ref="R33:T33" si="6" xml:space="preserve"> ABS(R9-R17)</f>
         <v>9.000000000000008E-3</v>
       </c>
       <c r="S33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.14099999999999996</v>
       </c>
       <c r="T33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.6000000000000059E-2</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="3"/>
+      <c r="A34" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>0.496</v>
+      </c>
+      <c r="G34" s="18">
+        <f xml:space="preserve"> AVERAGE(C34:F34)</f>
+        <v>0.4916666666666667</v>
+      </c>
       <c r="I34" s="2"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="J34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="16">
+        <v>0.27445109780439098</v>
+      </c>
+      <c r="L34" s="16">
+        <v>0.370259481037924</v>
+      </c>
+      <c r="M34" s="16">
+        <v>0.35528942115768403</v>
+      </c>
+      <c r="N34" s="21"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="1">
         <v>0.4</v>
       </c>
       <c r="R34" s="1">
-        <f t="shared" ref="R34:T34" si="4" xml:space="preserve"> ABS(R10-R18)</f>
+        <f t="shared" ref="R34:T34" si="7" xml:space="preserve"> ABS(R10-R18)</f>
         <v>4.0999999999999925E-2</v>
       </c>
       <c r="S34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.10799999999999998</v>
       </c>
       <c r="T34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.2999999999999918E-2</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="3"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="G35" s="18">
+        <f t="shared" ref="G35:G41" si="8" xml:space="preserve"> AVERAGE(C35:F35)</f>
+        <v>0.50900000000000001</v>
+      </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0.28443113772454998</v>
+      </c>
+      <c r="L35" s="16">
+        <v>0.380239520958083</v>
+      </c>
+      <c r="M35" s="16">
+        <v>0.33532934131736503</v>
+      </c>
+      <c r="N35" s="21"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="1">
         <v>0.5</v>
       </c>
       <c r="R35" s="1">
-        <f t="shared" ref="R35:T35" si="5" xml:space="preserve"> ABS(R11-R19)</f>
+        <f t="shared" ref="R35:T35" si="9" xml:space="preserve"> ABS(R11-R19)</f>
         <v>3.3999999999999919E-2</v>
       </c>
       <c r="S35" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.3999999999999919E-2</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="3"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.495</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="G36" s="18">
+        <f t="shared" si="8"/>
+        <v>0.5136666666666666</v>
+      </c>
       <c r="I36" s="2"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
+      <c r="J36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="16">
+        <v>0.28443113772454998</v>
+      </c>
+      <c r="L36" s="16">
+        <v>0.36227544910179599</v>
+      </c>
+      <c r="M36" s="16">
+        <v>0.35329341317365198</v>
+      </c>
+      <c r="N36" s="21"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="G37" s="3"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="3">
+        <v>0.497</v>
+      </c>
+      <c r="G37" s="18">
+        <f t="shared" si="8"/>
+        <v>0.49199999999999999</v>
+      </c>
       <c r="I37" s="2"/>
+      <c r="J37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="16">
+        <v>0.27844311377245501</v>
+      </c>
+      <c r="L37" s="16">
+        <v>0.380239520958083</v>
+      </c>
+      <c r="M37" s="16">
+        <v>0.34131736526946099</v>
+      </c>
+      <c r="N37" s="22"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="G38" s="3"/>
+      <c r="A38" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="18">
+        <f t="shared" si="8"/>
+        <v>0.496</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" s="18">
+        <f xml:space="preserve"> AVERAGE(K34:K37)</f>
+        <v>0.28043912175648644</v>
+      </c>
+      <c r="L38" s="18">
+        <f t="shared" ref="L38:M38" si="10" xml:space="preserve"> AVERAGE(L34:L37)</f>
+        <v>0.37325349301397148</v>
+      </c>
+      <c r="M38" s="18">
+        <f t="shared" si="10"/>
+        <v>0.34630738522954052</v>
+      </c>
+      <c r="N38" s="22"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A39" s="14"/>
+      <c r="B39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="18">
+        <f t="shared" si="8"/>
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="13"/>
-      <c r="S39" s="13"/>
-      <c r="T39" s="13"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A40" s="14"/>
+      <c r="B40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.502</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.496</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="18">
+        <f t="shared" si="8"/>
+        <v>0.49633333333333329</v>
+      </c>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="13"/>
-      <c r="V40" s="13"/>
-      <c r="W40" s="13"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.503</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="18">
+        <f t="shared" si="8"/>
+        <v>0.504</v>
+      </c>
       <c r="T41" s="1"/>
-      <c r="U41" s="13"/>
-      <c r="V41" s="13"/>
-      <c r="W41" s="13"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="T42" s="1"/>
-      <c r="U42" s="13"/>
-      <c r="V42" s="13"/>
-      <c r="W42" s="13"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="T43" s="1"/>
-      <c r="U43" s="13"/>
-      <c r="V43" s="13"/>
-      <c r="W43" s="13"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="13"/>
+      <c r="C45" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="10"/>
+      <c r="D45" s="13"/>
+      <c r="F45" t="s">
+        <v>33</v>
+      </c>
+      <c r="I45" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="3">
         <v>0.38300000000000001</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="3">
         <v>0.317</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="3">
+        <v>10.816000000000001</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="3">
         <v>0.317</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="3">
         <v>0.317</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>5.66</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="1">
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="3">
         <v>0.3</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="3">
         <v>0.36699999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+      <c r="F48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="3">
+        <v>15.231</v>
+      </c>
+      <c r="I48" s="14"/>
+      <c r="J48" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10" t="s">
+      <c r="B49" s="13"/>
+      <c r="C49" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="13"/>
+      <c r="F49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G49" s="3">
+        <v>171.31200000000001</v>
+      </c>
+      <c r="I49" s="14"/>
+      <c r="J49" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K49" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="3">
         <v>0.217</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="3">
         <v>0.26700000000000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" s="3">
+        <v>208.261</v>
+      </c>
+      <c r="I50" s="14"/>
+      <c r="J50" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="3">
         <v>0.38300000000000001</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="3">
         <v>0.41699999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F51" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="3">
+        <v>78.938000000000002</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="3">
         <v>0.4</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="3">
         <v>0.317</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
+      <c r="F52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="3">
+        <v>66.731999999999999</v>
+      </c>
+      <c r="I52" s="14"/>
+      <c r="J52" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10" t="s">
+      <c r="B53" s="13"/>
+      <c r="C53" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="13"/>
+      <c r="F53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" s="3">
+        <v>24.963999999999999</v>
+      </c>
+      <c r="I53" s="14"/>
+      <c r="J53" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="3">
         <v>0.33300000000000002</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="3">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="3">
+        <v>26.977</v>
+      </c>
+      <c r="I54" s="14"/>
+      <c r="J54" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="3">
         <v>0.3</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="3">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I55" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="3">
         <v>0.36699999999999999</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="3">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I56" s="14"/>
+      <c r="J56" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="C57" s="4"/>
       <c r="D57" s="1"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K57" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I58" s="14"/>
+      <c r="J58" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I59" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I60" s="14"/>
+      <c r="J60" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I61" s="14"/>
+      <c r="J61" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I62" s="14"/>
+      <c r="J62" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I63" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I64" s="14"/>
+      <c r="J64" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K64" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I65" s="14"/>
+      <c r="J65" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I66" s="14"/>
+      <c r="J66" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K66" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I67" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J67" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I68" s="14"/>
+      <c r="J68" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I69" s="14"/>
+      <c r="J69" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I70" s="14"/>
+      <c r="J70" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K70" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I71" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I72" s="14"/>
+      <c r="J72" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K72" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I73" s="14"/>
+      <c r="J73" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K73" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I74" s="14"/>
+      <c r="J74" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K74" s="1">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A22:A25"/>
+  <mergeCells count="25">
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="I71:I74"/>
+    <mergeCell ref="I47:I50"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="Q37:T37"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="C53:D53"/>
-    <mergeCell ref="Q37:T37"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update final set of data
</commit_message>
<xml_diff>
--- a/second-semester/src/data analyse.xlsx
+++ b/second-semester/src/data analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungh\Desktop\msc-project\second-semester\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1408F655-9C36-47C1-94CA-2F63B582858A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E332114-705C-4795-A6F8-93A031D943EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="-21600" windowWidth="19380" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="36">
   <si>
     <t>Move</t>
   </si>
@@ -178,24 +178,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -210,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,13 +216,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -244,8 +226,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -253,28 +238,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D33FE-1D44-4ACB-8B96-6B9822BF387F}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +567,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="5"/>
@@ -609,15 +577,15 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="1"/>
       <c r="J4" s="5" t="s">
         <v>20</v>
@@ -649,7 +617,7 @@
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="1"/>
@@ -665,52 +633,52 @@
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="15" t="s">
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
         <v>0.46700000000000003</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="3">
         <v>0.45800000000000002</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="3">
         <v>0.52100000000000002</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="3">
         <v>0.54300000000000004</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="11">
         <f xml:space="preserve"> AVERAGE(C6:G6)</f>
         <v>0.49725000000000008</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="16">
-        <v>0.29640718562874202</v>
-      </c>
-      <c r="L6" s="16">
-        <v>0.34131736526946099</v>
-      </c>
-      <c r="M6" s="16">
-        <v>0.36227544910179599</v>
-      </c>
-      <c r="N6" s="20"/>
+      <c r="K6" s="3">
+        <v>0.28542914171656603</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.36526946107784403</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.349301397205588</v>
+      </c>
+      <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="1" t="s">
@@ -729,40 +697,40 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
         <v>0.45400000000000001</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="3">
         <v>0.46500000000000002</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="3">
         <v>0.52500000000000002</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="3">
         <v>0.54300000000000004</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="11">
         <f t="shared" ref="H7:H24" si="0" xml:space="preserve"> AVERAGE(C7:G7)</f>
         <v>0.49675000000000002</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="16">
-        <v>0.28343313373253398</v>
-      </c>
-      <c r="L7" s="16">
-        <v>0.380239520958083</v>
-      </c>
-      <c r="M7" s="16">
-        <v>0.33632734530938102</v>
-      </c>
-      <c r="N7" s="20"/>
+      <c r="K7" s="3">
+        <v>0.26347305389221498</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.35229540918163599</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.38423153692614698</v>
+      </c>
+      <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="1">
@@ -781,40 +749,40 @@
       <c r="V7" s="1"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
         <v>0.45100000000000001</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="3">
         <v>0.46300000000000002</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="3">
         <v>0.50600000000000001</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="3">
         <v>0.50900000000000001</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="11">
         <f t="shared" si="0"/>
         <v>0.48224999999999996</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="16">
-        <v>0.29441117764470998</v>
-      </c>
-      <c r="L8" s="16">
-        <v>0.370259481037924</v>
-      </c>
-      <c r="M8" s="16">
-        <v>0.33532934131736503</v>
-      </c>
-      <c r="N8" s="20"/>
+      <c r="K8" s="3">
+        <v>0.29540918163672603</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.36526946107784403</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.339321357285429</v>
+      </c>
+      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="1">
@@ -833,46 +801,46 @@
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <v>0.44</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="3">
         <v>0.442</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="3">
         <v>0.52900000000000003</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="3">
         <v>0.54200000000000004</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="11">
         <f t="shared" si="0"/>
         <v>0.48825000000000002</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="16">
-        <v>0.29840319361277401</v>
-      </c>
-      <c r="L9" s="16">
-        <v>0.33133732534930099</v>
-      </c>
-      <c r="M9" s="16">
-        <v>0.370259481037924</v>
-      </c>
-      <c r="N9" s="20"/>
+      <c r="K9" s="3">
+        <v>0.269461077844311</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.37724550898203502</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.35329341317365198</v>
+      </c>
+      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="1">
         <v>0.3</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R9" s="16">
         <v>0.54200000000000004</v>
       </c>
       <c r="S9" s="1">
@@ -885,44 +853,44 @@
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="3">
         <v>0.53300000000000003</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="F10" s="16">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="F10" s="3">
         <v>0.56499999999999995</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="3">
         <v>0.56799999999999995</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>0.54449999999999998</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="11">
         <f xml:space="preserve"> AVERAGE(K6:K9)</f>
-        <v>0.29316367265469001</v>
-      </c>
-      <c r="L10" s="23">
+        <v>0.27844311377245451</v>
+      </c>
+      <c r="L10" s="11">
         <f t="shared" ref="L10:M10" si="1" xml:space="preserve"> AVERAGE(L6:L9)</f>
-        <v>0.35578842315369225</v>
-      </c>
-      <c r="M10" s="23">
+        <v>0.36501996007983978</v>
+      </c>
+      <c r="M10" s="11">
         <f t="shared" si="1"/>
-        <v>0.35104790419161652</v>
+        <v>0.35653692614770399</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -940,33 +908,33 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="3">
         <v>0.54600000000000004</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16">
-        <v>0.505</v>
-      </c>
-      <c r="F11" s="16">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <v>0.497</v>
+      </c>
+      <c r="F11" s="3">
         <v>0.58399999999999996</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="3">
         <v>0.53900000000000003</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>0.54350000000000009</v>
+        <v>0.54150000000000009</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="20"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="1">
@@ -983,126 +951,126 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="3">
         <v>0.54900000000000004</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="F12" s="16">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="F12" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="3">
         <v>0.57899999999999996</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>0.54875000000000007</v>
+        <v>0.54549999999999998</v>
       </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="20"/>
+      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="3">
         <v>0.55600000000000005</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="F13" s="16">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="F13" s="3">
         <v>0.57699999999999996</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="3">
         <v>0.59299999999999997</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="11">
         <f t="shared" si="0"/>
-        <v>0.56025000000000003</v>
+        <v>0.55925000000000002</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="3">
         <v>0.30738522954091801</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="3">
         <v>0.40219560878243499</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="3">
         <v>0.290419161676646</v>
       </c>
-      <c r="N13" s="20"/>
+      <c r="N13" s="3"/>
       <c r="O13" s="5"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="15" t="s">
+      <c r="Q13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="3">
         <v>0.54200000000000004</v>
       </c>
-      <c r="D14" s="16">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16">
+      <c r="D14" s="3">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
         <v>0.55400000000000005</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="3">
         <v>0.54100000000000004</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="11">
         <f t="shared" si="0"/>
-        <v>0.53125</v>
+        <v>0.53275000000000006</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="3">
         <v>0.30139720558882199</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="3">
         <v>0.41916167664670601</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="3">
         <v>0.279441117764471</v>
       </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
       <c r="Q14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1117,41 +1085,41 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="3">
         <v>0.53500000000000003</v>
       </c>
-      <c r="D15" s="16">
-        <v>0.495</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16">
+      <c r="D15" s="3">
+        <v>0.503</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
         <v>0.53200000000000003</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="3">
         <v>0.55300000000000005</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="11">
         <f t="shared" si="0"/>
-        <v>0.52875000000000005</v>
+        <v>0.53075000000000006</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="3">
         <v>0.30239520958083799</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="3">
         <v>0.37524950099800303</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="3">
         <v>0.32235528942115699</v>
       </c>
-      <c r="N15" s="20"/>
+      <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="1">
@@ -1168,41 +1136,41 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="3">
         <v>0.53700000000000003</v>
       </c>
-      <c r="D16" s="16">
-        <v>0.48299999999999998</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16">
+      <c r="D16" s="3">
+        <v>0.496</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
         <v>0.55700000000000005</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="3">
         <v>0.58699999999999997</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="11">
         <f t="shared" si="0"/>
-        <v>0.54099999999999993</v>
+        <v>0.5442499999999999</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="3">
         <v>0.319361277445109</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="3">
         <v>0.39321357285429098</v>
       </c>
-      <c r="M16" s="16">
+      <c r="M16" s="3">
         <v>0.28742514970059801</v>
       </c>
-      <c r="N16" s="20"/>
+      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="1">
@@ -1219,50 +1187,50 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="3">
         <v>0.55800000000000005</v>
       </c>
-      <c r="D17" s="16">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16">
+      <c r="D17" s="3">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="3">
         <v>0.53800000000000003</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="11">
         <f t="shared" si="0"/>
-        <v>0.53774999999999995</v>
+        <v>0.53875000000000006</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="24" t="s">
+      <c r="J17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="11">
         <f xml:space="preserve"> AVERAGE(K13:K16)</f>
         <v>0.30763473053892176</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="11">
         <f t="shared" ref="L17:M17" si="2" xml:space="preserve"> AVERAGE(L13:L16)</f>
         <v>0.39745508982035871</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="11">
         <f t="shared" si="2"/>
         <v>0.29491017964071797</v>
       </c>
-      <c r="N17" s="20"/>
+      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="1">
         <v>0.3</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R17" s="16">
         <v>0.53300000000000003</v>
       </c>
       <c r="S17" s="1">
@@ -1273,35 +1241,35 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="3">
         <v>0.47899999999999998</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="3">
         <v>0.435</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="3">
         <v>0.44600000000000001</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
         <v>0.51300000000000001</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="11">
         <f t="shared" si="0"/>
         <v>0.46824999999999994</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="20"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="1">
@@ -1318,39 +1286,39 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="3">
         <v>0.47499999999999998</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="3">
         <v>0.41599999999999998</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="3">
         <v>0.46800000000000003</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3">
         <v>0.51400000000000001</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="11">
         <f t="shared" si="0"/>
         <v>0.46825</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M19" s="19" t="s">
+      <c r="M19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N19" s="20"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="1">
@@ -1367,24 +1335,24 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="3">
         <v>0.49399999999999999</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="3">
         <v>0.45</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="3">
         <v>0.443</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
         <v>0.51</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="11">
         <f t="shared" si="0"/>
         <v>0.47425</v>
       </c>
@@ -1392,55 +1360,55 @@
       <c r="J20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="3">
         <v>0.33532934131736503</v>
       </c>
-      <c r="L20" s="16">
+      <c r="L20" s="3">
         <v>0.390219560878243</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="3">
         <v>0.27445109780439098</v>
       </c>
-      <c r="N20" s="20"/>
+      <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="3">
         <v>0.47399999999999998</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="3">
         <v>0.42299999999999999</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="3">
         <v>0.43</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
         <v>0.48299999999999998</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="11">
         <f t="shared" si="0"/>
         <v>0.45250000000000001</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="3">
         <v>0.300399201596806</v>
       </c>
-      <c r="L21" s="16">
+      <c r="L21" s="3">
         <v>0.42115768463073799</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M21" s="3">
         <v>0.27844311377245501</v>
       </c>
-      <c r="N21" s="20"/>
-      <c r="O21" s="10"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="8"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
@@ -1448,26 +1416,26 @@
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="1">
         <v>0.45700000000000002</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="1">
         <v>0.432</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="1">
         <v>0.45900000000000002</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="1">
         <v>0.48699999999999999</v>
       </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="18">
+      <c r="G22" s="1"/>
+      <c r="H22" s="11">
         <f t="shared" si="0"/>
         <v>0.45874999999999999</v>
       </c>
@@ -1475,16 +1443,16 @@
       <c r="J22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="16">
+      <c r="K22" s="3">
         <v>0.35828343313373201</v>
       </c>
-      <c r="L22" s="16">
+      <c r="L22" s="3">
         <v>0.38822355289421101</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="3">
         <v>0.25349301397205498</v>
       </c>
-      <c r="N22" s="20"/>
+      <c r="N22" s="3"/>
       <c r="O22" s="5"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="1"/>
@@ -1493,24 +1461,24 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="1">
         <v>0.45700000000000002</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="1">
         <v>0.46100000000000002</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="1">
         <v>0.48599999999999999</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="18">
+      <c r="G23" s="3"/>
+      <c r="H23" s="11">
         <f t="shared" si="0"/>
         <v>0.46274999999999999</v>
       </c>
@@ -1518,62 +1486,62 @@
       <c r="J23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="16">
+      <c r="K23" s="3">
         <v>0.29940119760479</v>
       </c>
-      <c r="L23" s="16">
+      <c r="L23" s="3">
         <v>0.40618762475049902</v>
       </c>
-      <c r="M23" s="16">
+      <c r="M23" s="3">
         <v>0.29441117764470998</v>
       </c>
-      <c r="N23" s="20"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="1">
         <v>0.49099999999999999</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="1">
         <v>0.42099999999999999</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="1">
         <v>0.41299999999999998</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="1">
         <v>0.49</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="18">
+      <c r="G24" s="3"/>
+      <c r="H24" s="11">
         <f t="shared" si="0"/>
         <v>0.45374999999999999</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="11">
         <f xml:space="preserve"> AVERAGE(K20:K23)</f>
         <v>0.32335329341317326</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="11">
         <f xml:space="preserve"> AVERAGE(L20:L23)</f>
         <v>0.40144710578842274</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="11">
         <f xml:space="preserve"> AVERAGE(M20:M23)</f>
         <v>0.27519960079840278</v>
       </c>
-      <c r="N24" s="20"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="1"/>
@@ -1582,24 +1550,24 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="1">
         <v>0.45800000000000002</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="1">
         <v>0.40699999999999997</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="1">
         <v>0.46200000000000002</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="1">
         <v>0.51700000000000002</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="18">
+      <c r="G25" s="3"/>
+      <c r="H25" s="11">
         <f xml:space="preserve"> AVERAGE(C25:G25)</f>
         <v>0.46099999999999997</v>
       </c>
@@ -1608,7 +1576,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="20"/>
+      <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="1"/>
@@ -1633,7 +1601,7 @@
       <c r="M26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N26" s="20"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="1"/>
@@ -1651,16 +1619,16 @@
       <c r="J27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="16">
+      <c r="K27" s="3">
         <v>0.30339321357285398</v>
       </c>
-      <c r="L27" s="16">
+      <c r="L27" s="3">
         <v>0.37125748502993999</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27" s="3">
         <v>0.32534930139720503</v>
       </c>
-      <c r="N27" s="20"/>
+      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="1"/>
@@ -1674,16 +1642,16 @@
       <c r="J28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="16">
+      <c r="K28" s="3">
         <v>0.300399201596806</v>
       </c>
-      <c r="L28" s="16">
+      <c r="L28" s="3">
         <v>0.36826347305389201</v>
       </c>
-      <c r="M28" s="16">
+      <c r="M28" s="3">
         <v>0.33133732534930099</v>
       </c>
-      <c r="N28" s="20"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
     </row>
@@ -1693,16 +1661,16 @@
       <c r="J29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="16">
+      <c r="K29" s="3">
         <v>0.249500998003992</v>
       </c>
-      <c r="L29" s="16">
+      <c r="L29" s="3">
         <v>0.40818363273453001</v>
       </c>
-      <c r="M29" s="16">
+      <c r="M29" s="3">
         <v>0.34231536926147699</v>
       </c>
-      <c r="N29" s="20"/>
+      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
@@ -1711,30 +1679,22 @@
       <c r="J30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K30" s="16">
+      <c r="K30" s="3">
         <v>0.31536926147704503</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L30" s="3">
         <v>0.35628742514970002</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="3">
         <v>0.32834331337325301</v>
       </c>
-      <c r="N30" s="20"/>
-      <c r="O30" s="10"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="8"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R30" s="1">
-        <v>1</v>
-      </c>
-      <c r="S30" s="1">
-        <v>3</v>
-      </c>
-      <c r="T30" s="1">
-        <v>5</v>
-      </c>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C31" s="5"/>
@@ -1743,73 +1703,51 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="24" t="s">
+      <c r="J31" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K31" s="11">
         <f xml:space="preserve"> AVERAGE(K27:K30)</f>
         <v>0.29216566866267424</v>
       </c>
-      <c r="L31" s="23">
+      <c r="L31" s="11">
         <f t="shared" ref="L31:M31" si="3" xml:space="preserve"> AVERAGE(L27:L30)</f>
         <v>0.37599800399201555</v>
       </c>
-      <c r="M31" s="23">
+      <c r="M31" s="11">
         <f t="shared" si="3"/>
         <v>0.33183632734530899</v>
       </c>
-      <c r="N31" s="20"/>
+      <c r="N31" s="3"/>
       <c r="O31" s="5"/>
       <c r="P31" s="6"/>
-      <c r="Q31" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="R31" s="1">
-        <f xml:space="preserve"> ABS(R7-R15)</f>
-        <v>0.14200000000000002</v>
-      </c>
-      <c r="S31" s="1">
-        <f t="shared" ref="S31:T31" si="4" xml:space="preserve"> ABS(S7-S15)</f>
-        <v>1.7000000000000015E-2</v>
-      </c>
-      <c r="T31" s="1">
-        <f t="shared" si="4"/>
-        <v>0.19199999999999995</v>
-      </c>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="17"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="5"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="R32" s="1">
-        <f t="shared" ref="R32:T32" si="5" xml:space="preserve"> ABS(R8-R16)</f>
-        <v>6.6999999999999948E-2</v>
-      </c>
-      <c r="S32" s="1">
-        <f t="shared" si="5"/>
-        <v>2.4999999999999967E-2</v>
-      </c>
-      <c r="T32" s="1">
-        <f t="shared" si="5"/>
-        <v>6.6000000000000003E-2</v>
-      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
@@ -1827,7 +1765,7 @@
       <c r="F33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I33" s="2"/>
@@ -1841,30 +1779,19 @@
       <c r="M33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N33" s="20"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="R33" s="7">
-        <f t="shared" ref="R33:T33" si="6" xml:space="preserve"> ABS(R9-R17)</f>
-        <v>9.000000000000008E-3</v>
-      </c>
-      <c r="S33" s="1">
-        <f t="shared" si="6"/>
-        <v>0.14099999999999996</v>
-      </c>
-      <c r="T33" s="1">
-        <f t="shared" si="6"/>
-        <v>6.6000000000000059E-2</v>
-      </c>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="3">
@@ -1877,7 +1804,7 @@
       <c r="F34" s="3">
         <v>0.496</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="11">
         <f xml:space="preserve"> AVERAGE(C34:F34)</f>
         <v>0.4916666666666667</v>
       </c>
@@ -1885,37 +1812,26 @@
       <c r="J34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="16">
+      <c r="K34" s="3">
         <v>0.27445109780439098</v>
       </c>
-      <c r="L34" s="16">
+      <c r="L34" s="3">
         <v>0.370259481037924</v>
       </c>
-      <c r="M34" s="16">
+      <c r="M34" s="3">
         <v>0.35528942115768403</v>
       </c>
-      <c r="N34" s="21"/>
+      <c r="N34" s="1"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="R34" s="1">
-        <f t="shared" ref="R34:T34" si="7" xml:space="preserve"> ABS(R10-R18)</f>
-        <v>4.0999999999999925E-2</v>
-      </c>
-      <c r="S34" s="1">
-        <f t="shared" si="7"/>
-        <v>0.10799999999999998</v>
-      </c>
-      <c r="T34" s="1">
-        <f t="shared" si="7"/>
-        <v>3.2999999999999918E-2</v>
-      </c>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="13"/>
+      <c r="B35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="3">
@@ -1928,45 +1844,34 @@
       <c r="F35" s="3">
         <v>0.52500000000000002</v>
       </c>
-      <c r="G35" s="18">
-        <f t="shared" ref="G35:G41" si="8" xml:space="preserve"> AVERAGE(C35:F35)</f>
+      <c r="G35" s="11">
+        <f t="shared" ref="G35:G41" si="4" xml:space="preserve"> AVERAGE(C35:F35)</f>
         <v>0.50900000000000001</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="16">
+      <c r="K35" s="3">
         <v>0.28443113772454998</v>
       </c>
-      <c r="L35" s="16">
+      <c r="L35" s="3">
         <v>0.380239520958083</v>
       </c>
-      <c r="M35" s="16">
+      <c r="M35" s="3">
         <v>0.33532934131736503</v>
       </c>
-      <c r="N35" s="21"/>
+      <c r="N35" s="1"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="R35" s="1">
-        <f t="shared" ref="R35:T35" si="9" xml:space="preserve"> ABS(R11-R19)</f>
-        <v>3.3999999999999919E-2</v>
-      </c>
-      <c r="S35" s="7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="T35" s="1">
-        <f t="shared" si="9"/>
-        <v>3.3999999999999919E-2</v>
-      </c>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="11" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="3">
@@ -1979,30 +1884,30 @@
       <c r="F36" s="3">
         <v>0.504</v>
       </c>
-      <c r="G36" s="18">
-        <f t="shared" si="8"/>
+      <c r="G36" s="11">
+        <f t="shared" si="4"/>
         <v>0.5136666666666666</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K36" s="16">
+      <c r="K36" s="3">
         <v>0.28443113772454998</v>
       </c>
-      <c r="L36" s="16">
+      <c r="L36" s="3">
         <v>0.36227544910179599</v>
       </c>
-      <c r="M36" s="16">
+      <c r="M36" s="3">
         <v>0.35329341317365198</v>
       </c>
-      <c r="N36" s="21"/>
+      <c r="N36" s="1"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="11" t="s">
+      <c r="A37" s="13"/>
+      <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="3">
@@ -2011,40 +1916,39 @@
       <c r="D37" s="3">
         <v>0.47099999999999997</v>
       </c>
-      <c r="E37" s="10"/>
+      <c r="E37" s="8"/>
       <c r="F37" s="3">
         <v>0.497</v>
       </c>
-      <c r="G37" s="18">
-        <f t="shared" si="8"/>
+      <c r="G37" s="11">
+        <f t="shared" si="4"/>
         <v>0.49199999999999999</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K37" s="16">
+      <c r="K37" s="3">
         <v>0.27844311377245501</v>
       </c>
-      <c r="L37" s="16">
+      <c r="L37" s="3">
         <v>0.380239520958083</v>
       </c>
-      <c r="M37" s="16">
+      <c r="M37" s="3">
         <v>0.34131736526946099</v>
       </c>
-      <c r="N37" s="22"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3">
@@ -2057,34 +1961,33 @@
         <v>0.504</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="18">
-        <f t="shared" si="8"/>
+      <c r="G38" s="11">
+        <f t="shared" si="4"/>
         <v>0.496</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="J38" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="11">
         <f xml:space="preserve"> AVERAGE(K34:K37)</f>
         <v>0.28043912175648644</v>
       </c>
-      <c r="L38" s="18">
-        <f t="shared" ref="L38:M38" si="10" xml:space="preserve"> AVERAGE(L34:L37)</f>
+      <c r="L38" s="11">
+        <f t="shared" ref="L38:M38" si="5" xml:space="preserve"> AVERAGE(L34:L37)</f>
         <v>0.37325349301397148</v>
       </c>
-      <c r="M38" s="18">
-        <f t="shared" si="10"/>
+      <c r="M38" s="11">
+        <f t="shared" si="5"/>
         <v>0.34630738522954052</v>
       </c>
-      <c r="N38" s="22"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="13"/>
+      <c r="B39" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="3">
@@ -2097,8 +2000,8 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="18">
-        <f t="shared" si="8"/>
+      <c r="G39" s="11">
+        <f t="shared" si="4"/>
         <v>0.4916666666666667</v>
       </c>
       <c r="J39" s="1"/>
@@ -2111,8 +2014,8 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="13"/>
+      <c r="B40" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="3">
@@ -2125,8 +2028,8 @@
         <v>0.496</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="18">
-        <f t="shared" si="8"/>
+      <c r="G40" s="11">
+        <f t="shared" si="4"/>
         <v>0.49633333333333329</v>
       </c>
       <c r="J40" s="1"/>
@@ -2139,8 +2042,8 @@
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="11" t="s">
+      <c r="A41" s="13"/>
+      <c r="B41" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="3">
@@ -2153,8 +2056,8 @@
         <v>0.503</v>
       </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="18">
-        <f t="shared" si="8"/>
+      <c r="G41" s="11">
+        <f t="shared" si="4"/>
         <v>0.504</v>
       </c>
       <c r="T41" s="1"/>
@@ -2175,14 +2078,14 @@
       <c r="W43" s="1"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13" t="s">
+      <c r="B45" s="15"/>
+      <c r="C45" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="13"/>
+      <c r="D45" s="15"/>
       <c r="F45" t="s">
         <v>33</v>
       </c>
@@ -2235,14 +2138,14 @@
       <c r="G47" s="3">
         <v>5.66</v>
       </c>
-      <c r="I47" s="14" t="s">
+      <c r="I47" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J47" s="11" t="s">
+      <c r="J47" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K47" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
@@ -2264,35 +2167,35 @@
       <c r="G48" s="3">
         <v>15.231</v>
       </c>
-      <c r="I48" s="14"/>
-      <c r="J48" s="11" t="s">
+      <c r="I48" s="13"/>
+      <c r="J48" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K48" s="1">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="13"/>
+      <c r="D49" s="15"/>
       <c r="F49" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G49" s="3">
         <v>171.31200000000001</v>
       </c>
-      <c r="I49" s="14"/>
-      <c r="J49" s="11" t="s">
+      <c r="I49" s="13"/>
+      <c r="J49" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K49" s="1">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -2314,12 +2217,12 @@
       <c r="G50" s="3">
         <v>208.261</v>
       </c>
-      <c r="I50" s="14"/>
-      <c r="J50" s="11" t="s">
+      <c r="I50" s="13"/>
+      <c r="J50" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K50" s="1">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -2341,14 +2244,14 @@
       <c r="G51" s="3">
         <v>78.938000000000002</v>
       </c>
-      <c r="I51" s="14" t="s">
+      <c r="I51" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J51" s="11" t="s">
+      <c r="J51" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K51" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
@@ -2370,35 +2273,35 @@
       <c r="G52" s="3">
         <v>66.731999999999999</v>
       </c>
-      <c r="I52" s="14"/>
-      <c r="J52" s="11" t="s">
+      <c r="I52" s="13"/>
+      <c r="J52" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K52" s="1">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13" t="s">
+      <c r="B53" s="15"/>
+      <c r="C53" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="13"/>
+      <c r="D53" s="15"/>
       <c r="F53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G53" s="3">
         <v>24.963999999999999</v>
       </c>
-      <c r="I53" s="14"/>
-      <c r="J53" s="11" t="s">
+      <c r="I53" s="13"/>
+      <c r="J53" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K53" s="1">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -2420,12 +2323,12 @@
       <c r="G54" s="3">
         <v>26.977</v>
       </c>
-      <c r="I54" s="14"/>
-      <c r="J54" s="11" t="s">
+      <c r="I54" s="13"/>
+      <c r="J54" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K54" s="1">
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -2441,14 +2344,14 @@
       <c r="D55" s="3">
         <v>0.4</v>
       </c>
-      <c r="I55" s="14" t="s">
+      <c r="I55" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J55" s="11" t="s">
+      <c r="J55" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K55" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -2464,12 +2367,12 @@
       <c r="D56" s="3">
         <v>0.35</v>
       </c>
-      <c r="I56" s="14"/>
-      <c r="J56" s="11" t="s">
+      <c r="I56" s="13"/>
+      <c r="J56" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K56" s="1">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -2477,28 +2380,28 @@
       <c r="B57" s="1"/>
       <c r="C57" s="4"/>
       <c r="D57" s="1"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="11" t="s">
+      <c r="I57" s="13"/>
+      <c r="J57" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K57" s="1">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I58" s="14"/>
-      <c r="J58" s="11" t="s">
+      <c r="I58" s="13"/>
+      <c r="J58" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K58" s="1">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I59" s="14" t="s">
+      <c r="I59" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J59" s="11" t="s">
+      <c r="J59" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K59" s="1">
@@ -2506,8 +2409,8 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I60" s="14"/>
-      <c r="J60" s="11" t="s">
+      <c r="I60" s="13"/>
+      <c r="J60" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K60" s="1">
@@ -2515,8 +2418,8 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I61" s="14"/>
-      <c r="J61" s="11" t="s">
+      <c r="I61" s="13"/>
+      <c r="J61" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K61" s="1">
@@ -2524,8 +2427,8 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I62" s="14"/>
-      <c r="J62" s="11" t="s">
+      <c r="I62" s="13"/>
+      <c r="J62" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K62" s="1">
@@ -2533,19 +2436,19 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I63" s="14" t="s">
+      <c r="I63" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J63" s="11" t="s">
+      <c r="J63" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I64" s="14"/>
-      <c r="J64" s="11" t="s">
+      <c r="I64" s="13"/>
+      <c r="J64" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K64" s="1">
@@ -2553,8 +2456,8 @@
       </c>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I65" s="14"/>
-      <c r="J65" s="11" t="s">
+      <c r="I65" s="13"/>
+      <c r="J65" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K65" s="1">
@@ -2562,8 +2465,8 @@
       </c>
     </row>
     <row r="66" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I66" s="14"/>
-      <c r="J66" s="11" t="s">
+      <c r="I66" s="13"/>
+      <c r="J66" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K66" s="1">
@@ -2571,90 +2474,89 @@
       </c>
     </row>
     <row r="67" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I67" s="14" t="s">
+      <c r="I67" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J67" s="11" t="s">
+      <c r="J67" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K67" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I68" s="13"/>
+      <c r="J68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I69" s="13"/>
+      <c r="J69" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I70" s="13"/>
+      <c r="J70" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K70" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I71" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I68" s="14"/>
-      <c r="J68" s="11" t="s">
+    <row r="72" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I72" s="13"/>
+      <c r="J72" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K68" s="1">
+      <c r="K72" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I69" s="14"/>
-      <c r="J69" s="11" t="s">
+    <row r="73" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I73" s="13"/>
+      <c r="J73" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K69" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I70" s="14"/>
-      <c r="J70" s="11" t="s">
+      <c r="K73" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I74" s="13"/>
+      <c r="J74" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K70" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I71" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J71" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K71" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I72" s="14"/>
-      <c r="J72" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K72" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I73" s="14"/>
-      <c r="J73" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K73" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="74" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I74" s="14"/>
-      <c r="J74" s="11" t="s">
-        <v>19</v>
-      </c>
       <c r="K74" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I67:I70"/>
-    <mergeCell ref="I71:I74"/>
-    <mergeCell ref="I47:I50"/>
-    <mergeCell ref="I51:I54"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="I59:I62"/>
-    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A32:F32"/>
     <mergeCell ref="Q37:T37"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="R5:U5"/>
@@ -2667,12 +2569,13 @@
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A38:A41"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="I71:I74"/>
+    <mergeCell ref="I47:I50"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="I63:I66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new experiment data
</commit_message>
<xml_diff>
--- a/second-semester/src/data analyse.xlsx
+++ b/second-semester/src/data analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungh\Desktop\msc-project\second-semester\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E332114-705C-4795-A6F8-93A031D943EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F596AB-1D14-4C48-A2A3-8C16C12FE769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9880" yWindow="-21600" windowWidth="19380" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
   <si>
     <t>Move</t>
   </si>
@@ -198,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,9 +239,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D33FE-1D44-4ACB-8B96-6B9822BF387F}">
-  <dimension ref="A1:W74"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
@@ -629,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="1"/>
@@ -840,7 +837,7 @@
       <c r="Q9" s="1">
         <v>0.3</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="1">
         <v>0.54200000000000004</v>
       </c>
       <c r="S9" s="1">
@@ -1033,7 +1030,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>16</v>
@@ -1230,7 +1227,7 @@
       <c r="Q17" s="1">
         <v>0.3</v>
       </c>
-      <c r="R17" s="16">
+      <c r="R17" s="1">
         <v>0.53300000000000003</v>
       </c>
       <c r="S17" s="1">
@@ -1620,13 +1617,13 @@
         <v>16</v>
       </c>
       <c r="K27" s="3">
-        <v>0.30339321357285398</v>
+        <v>0.28143712574850299</v>
       </c>
       <c r="L27" s="3">
-        <v>0.37125748502993999</v>
+        <v>0.389221556886227</v>
       </c>
       <c r="M27" s="3">
-        <v>0.32534930139720503</v>
+        <v>0.329341317365269</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -1643,13 +1640,13 @@
         <v>17</v>
       </c>
       <c r="K28" s="3">
-        <v>0.300399201596806</v>
+        <v>0.26447105788423098</v>
       </c>
       <c r="L28" s="3">
-        <v>0.36826347305389201</v>
+        <v>0.38522954091816303</v>
       </c>
       <c r="M28" s="3">
-        <v>0.33133732534930099</v>
+        <v>0.350299401197604</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -1662,13 +1659,13 @@
         <v>18</v>
       </c>
       <c r="K29" s="3">
-        <v>0.249500998003992</v>
+        <v>0.28642714570858202</v>
       </c>
       <c r="L29" s="3">
-        <v>0.40818363273453001</v>
+        <v>0.37325349301397198</v>
       </c>
       <c r="M29" s="3">
-        <v>0.34231536926147699</v>
+        <v>0.340319361277445</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -1680,21 +1677,21 @@
         <v>19</v>
       </c>
       <c r="K30" s="3">
-        <v>0.31536926147704503</v>
+        <v>0.25449101796407098</v>
       </c>
       <c r="L30" s="3">
-        <v>0.35628742514970002</v>
+        <v>0.41516966067864203</v>
       </c>
       <c r="M30" s="3">
-        <v>0.32834331337325301</v>
+        <v>0.330339321357285</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="8"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C31" s="5"/>
@@ -1708,23 +1705,23 @@
       </c>
       <c r="K31" s="11">
         <f xml:space="preserve"> AVERAGE(K27:K30)</f>
-        <v>0.29216566866267424</v>
+        <v>0.27170658682634674</v>
       </c>
       <c r="L31" s="11">
         <f t="shared" ref="L31:M31" si="3" xml:space="preserve"> AVERAGE(L27:L30)</f>
-        <v>0.37599800399201555</v>
+        <v>0.390718562874251</v>
       </c>
       <c r="M31" s="11">
         <f t="shared" si="3"/>
-        <v>0.33183632734530899</v>
+        <v>0.33757485029940076</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="5"/>
       <c r="P31" s="6"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
@@ -1744,12 +1741,12 @@
       <c r="N32" s="3"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
@@ -1760,15 +1757,17 @@
         <v>0</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I33" s="2"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
         <v>7</v>
@@ -1782,12 +1781,12 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>30</v>
       </c>
@@ -1795,147 +1794,155 @@
         <v>16</v>
       </c>
       <c r="C34" s="3">
-        <v>0.52200000000000002</v>
+        <v>0.52195608782435099</v>
       </c>
       <c r="D34" s="3">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3">
+        <v>0.47904191616766401</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.50299401197604698</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3">
         <v>0.496</v>
       </c>
-      <c r="G34" s="11">
-        <f xml:space="preserve"> AVERAGE(C34:F34)</f>
-        <v>0.4916666666666667</v>
-      </c>
-      <c r="I34" s="2"/>
+      <c r="H34" s="11">
+        <f xml:space="preserve"> AVERAGE(C34:G34)</f>
+        <v>0.49999800399201549</v>
+      </c>
       <c r="J34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K34" s="3">
-        <v>0.27445109780439098</v>
+        <v>0.31736526946107702</v>
       </c>
       <c r="L34" s="3">
-        <v>0.370259481037924</v>
+        <v>0.36227544910179599</v>
       </c>
       <c r="M34" s="3">
-        <v>0.35528942115768403</v>
+        <v>0.320359281437125</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="3">
-        <v>0.52600000000000002</v>
+        <v>0.52594810379241497</v>
       </c>
       <c r="D35" s="3">
-        <v>0.47599999999999998</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3">
+        <v>0.48403193612774398</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.45908183632734501</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3">
         <v>0.52500000000000002</v>
       </c>
-      <c r="G35" s="11">
-        <f t="shared" ref="G35:G41" si="4" xml:space="preserve"> AVERAGE(C35:F35)</f>
-        <v>0.50900000000000001</v>
-      </c>
-      <c r="I35" s="2"/>
+      <c r="H35" s="11">
+        <f t="shared" ref="H35:H41" si="4" xml:space="preserve"> AVERAGE(C35:G35)</f>
+        <v>0.49851546906187594</v>
+      </c>
       <c r="J35" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3">
-        <v>0.28443113772454998</v>
+        <v>0.29141716566866199</v>
       </c>
       <c r="L35" s="3">
-        <v>0.380239520958083</v>
+        <v>0.36327345309381198</v>
       </c>
       <c r="M35" s="3">
-        <v>0.33532934131736503</v>
+        <v>0.34530938123752403</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="3">
-        <v>0.54200000000000004</v>
+        <v>0.54191616766466999</v>
       </c>
       <c r="D36" s="3">
-        <v>0.495</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3">
+        <v>0.48902195608782401</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.49301397205588798</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3">
         <v>0.504</v>
       </c>
-      <c r="G36" s="11">
+      <c r="H36" s="11">
         <f t="shared" si="4"/>
-        <v>0.5136666666666666</v>
-      </c>
-      <c r="I36" s="2"/>
+        <v>0.50698802395209541</v>
+      </c>
       <c r="J36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K36" s="3">
-        <v>0.28443113772454998</v>
+        <v>0.28842315369261401</v>
       </c>
       <c r="L36" s="3">
-        <v>0.36227544910179599</v>
+        <v>0.38722554890219502</v>
       </c>
       <c r="M36" s="3">
-        <v>0.35329341317365198</v>
+        <v>0.32435129740518898</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="3">
-        <v>0.50800000000000001</v>
+        <v>0.50798403193612696</v>
       </c>
       <c r="D37" s="3">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="3">
+        <v>0.48502994011975997</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.47904191616766401</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="3">
         <v>0.497</v>
       </c>
-      <c r="G37" s="11">
+      <c r="H37" s="11">
         <f t="shared" si="4"/>
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="I37" s="2"/>
+        <v>0.49226397205588768</v>
+      </c>
       <c r="J37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K37" s="3">
-        <v>0.27844311377245501</v>
+        <v>0.30339321357285398</v>
       </c>
       <c r="L37" s="3">
-        <v>0.380239520958083</v>
+        <v>0.379241516966067</v>
       </c>
       <c r="M37" s="3">
-        <v>0.34131736526946099</v>
+        <v>0.31736526946107702</v>
       </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -1944,7 +1951,7 @@
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>31</v>
       </c>
@@ -1952,132 +1959,144 @@
         <v>16</v>
       </c>
       <c r="C38" s="3">
-        <v>0.52</v>
+        <v>0.519960079840319</v>
       </c>
       <c r="D38" s="3">
-        <v>0.46400000000000002</v>
+        <v>0.46407185628742498</v>
       </c>
       <c r="E38" s="3">
+        <v>0.50998003992015895</v>
+      </c>
+      <c r="F38" s="3">
         <v>0.504</v>
       </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="11">
+      <c r="G38" s="3"/>
+      <c r="H38" s="11">
         <f t="shared" si="4"/>
-        <v>0.496</v>
+        <v>0.49950299401197573</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>8</v>
       </c>
       <c r="K38" s="11">
         <f xml:space="preserve"> AVERAGE(K34:K37)</f>
-        <v>0.28043912175648644</v>
+        <v>0.30014970059880175</v>
       </c>
       <c r="L38" s="11">
         <f t="shared" ref="L38:M38" si="5" xml:space="preserve"> AVERAGE(L34:L37)</f>
-        <v>0.37325349301397148</v>
+        <v>0.37300399201596751</v>
       </c>
       <c r="M38" s="11">
         <f t="shared" si="5"/>
-        <v>0.34630738522954052</v>
+        <v>0.3268463073852288</v>
       </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="3">
-        <v>0.53</v>
+        <v>0.52994011976047894</v>
       </c>
       <c r="D39" s="3">
-        <v>0.47</v>
+        <v>0.47005988023952</v>
       </c>
       <c r="E39" s="3">
+        <v>0.46307385229540898</v>
+      </c>
+      <c r="F39" s="3">
         <v>0.47499999999999998</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="11">
+      <c r="G39" s="3"/>
+      <c r="H39" s="11">
         <f t="shared" si="4"/>
-        <v>0.4916666666666667</v>
-      </c>
-      <c r="J39" s="1"/>
+        <v>0.48451846307385193</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="N39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U39" s="1"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="3">
-        <v>0.502</v>
+        <v>0.50199600798403199</v>
       </c>
       <c r="D40" s="3">
-        <v>0.49099999999999999</v>
+        <v>0.46606786427145702</v>
       </c>
       <c r="E40" s="3">
+        <v>0.47205588822355199</v>
+      </c>
+      <c r="F40" s="3">
         <v>0.496</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="11">
+      <c r="G40" s="3"/>
+      <c r="H40" s="11">
         <f t="shared" si="4"/>
-        <v>0.49633333333333329</v>
-      </c>
-      <c r="J40" s="1"/>
+        <v>0.48402994011976025</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="T40" s="1"/>
+      <c r="N40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="3">
-        <v>0.52400000000000002</v>
+        <v>0.52395209580838298</v>
       </c>
       <c r="D41" s="3">
-        <v>0.48499999999999999</v>
+        <v>0.45708582834331302</v>
       </c>
       <c r="E41" s="3">
+        <v>0.47105788423153599</v>
+      </c>
+      <c r="F41" s="3">
         <v>0.503</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="11">
+      <c r="G41" s="3"/>
+      <c r="H41" s="11">
         <f t="shared" si="4"/>
-        <v>0.504</v>
-      </c>
-      <c r="T41" s="1"/>
+        <v>0.48877395209580798</v>
+      </c>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>10</v>
       </c>
@@ -2093,7 +2112,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2119,7 +2138,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -2148,7 +2167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>